<commit_message>
Test: add test cases for Normal theme
</commit_message>
<xml_diff>
--- a/PiratenKapern/src/test/java/test/game/Theme/theme test case.xlsx
+++ b/PiratenKapern/src/test/java/test/game/Theme/theme test case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Carleton\4004\a1\4004F2020-PiratenKapern\PiratenKapern\src\test\java\test\game\Theme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{129CCE3B-4E47-420E-B1F8-88F23F819528}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB32FC4-9545-4926-BC40-0D888C3AC16F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="4485" windowWidth="20730" windowHeight="11160" xr2:uid="{4453D95F-B99C-4EBC-BF1D-88ACF2A1429C}"/>
   </bookViews>
@@ -151,18 +151,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>no coin/diamond bouns</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>with coin/diamond bouns</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>coin/diamond oak + bouns</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>3oak+coinx3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -200,6 +188,18 @@
   </si>
   <si>
     <t>3oak+5oak+coinx8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no coin/diamond bonus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>with coin/diamond bonus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>coin/diamond oak + bonus</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -670,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F6EA3C4-DE68-497B-AA93-69DD73F51F1B}">
-  <dimension ref="A2:L33"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -682,69 +682,88 @@
     <col min="9" max="9" width="41.375" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" t="s">
+        <v>26</v>
+      </c>
+    </row>
     <row r="2" spans="1:12">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <f>SUM(A3:F3)</f>
+        <v>8</v>
+      </c>
+      <c r="H3">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8" t="s">
-        <v>30</v>
-      </c>
+      <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:12">
       <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G4">
-        <f>SUM(A4:F4)</f>
+        <f t="shared" ref="G4:G32" si="0">SUM(A4:F4)</f>
         <v>8</v>
       </c>
       <c r="H4">
@@ -754,32 +773,37 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
       </c>
       <c r="G5">
-        <f t="shared" ref="G5:G35" si="0">SUM(A5:F5)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1"/>
+        <v>100</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -789,10 +813,10 @@
         <v>8</v>
       </c>
       <c r="H6">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -800,23 +824,20 @@
         <v>2</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
       <c r="G7">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="H7">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -824,184 +845,187 @@
         <v>2</v>
       </c>
       <c r="B8">
-        <v>5</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="H8">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="H9">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10">
-        <v>1</v>
-      </c>
       <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H10">
+        <v>4000</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15" thickBot="1">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H12">
+        <v>300</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G10">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H10">
-        <v>2000</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="B11">
-        <v>8</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H11">
-        <v>4000</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="15" thickBot="1">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="9" t="s">
-        <v>31</v>
+      <c r="L12" s="3">
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13">
-        <v>1</v>
-      </c>
       <c r="B13">
-        <v>3</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G13">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="H13">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="L13" s="3">
-        <v>100</v>
+        <v>20</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L13" s="5">
+        <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="B14">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
       </c>
       <c r="E14">
         <v>2</v>
       </c>
-      <c r="F14">
-        <v>2</v>
-      </c>
       <c r="G14">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="H14">
-        <v>600</v>
+        <v>700</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L14" s="5">
-        <v>200</v>
+        <v>500</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="B15">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="H15">
-        <v>700</v>
+        <v>1100</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="L15" s="5">
-        <v>500</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="B16">
-        <v>6</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16">
+        <v>7</v>
+      </c>
+      <c r="F16">
         <v>1</v>
       </c>
       <c r="G16">
@@ -1009,99 +1033,93 @@
         <v>8</v>
       </c>
       <c r="H16">
-        <v>1100</v>
+        <v>2100</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="L16" s="5">
-        <v>1000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="B17">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F17">
         <v>1</v>
       </c>
       <c r="G17">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H17">
-        <v>2100</v>
+        <v>4100</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="L17" s="5">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15" thickBot="1">
+      <c r="A18">
+        <v>2</v>
+      </c>
       <c r="B18">
-        <v>8</v>
-      </c>
-      <c r="F18">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
       </c>
       <c r="G18">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H18">
-        <v>4100</v>
+        <v>200</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K18" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="L18" s="5">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="15" thickBot="1">
+        <v>27</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L18" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B19">
         <v>3</v>
       </c>
       <c r="C19">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G19">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="H19">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K19" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="L19" s="7" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20">
-        <v>1</v>
-      </c>
       <c r="B20">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C20">
         <v>4</v>
@@ -1111,41 +1129,47 @@
         <v>8</v>
       </c>
       <c r="H20">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:12">
-      <c r="B21">
-        <v>4</v>
-      </c>
-      <c r="C21">
-        <v>4</v>
-      </c>
-      <c r="G21">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H21">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="F22">
+        <v>3</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H22">
         <v>400</v>
       </c>
-      <c r="I21" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="9" t="s">
-        <v>32</v>
+      <c r="I22" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -1156,20 +1180,20 @@
         <v>2</v>
       </c>
       <c r="C23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G23">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="H23">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -1177,23 +1201,23 @@
         <v>1</v>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="F24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G24">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="H24">
-        <v>600</v>
+        <v>1000</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -1203,98 +1227,95 @@
       <c r="B25">
         <v>1</v>
       </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
       <c r="F25">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G25">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="H25">
-        <v>1000</v>
+        <v>1600</v>
       </c>
       <c r="I25" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>7</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H26">
+        <v>2700</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="F27">
+        <v>8</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H27">
+        <v>4800</v>
+      </c>
+      <c r="I27" s="1" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
-      <c r="A26">
-        <v>1</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="F26">
-        <v>6</v>
-      </c>
-      <c r="G26">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H26">
-        <v>1600</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12">
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="F27">
-        <v>7</v>
-      </c>
-      <c r="G27">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H27">
-        <v>2700</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:12">
       <c r="F28">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G28">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H28">
-        <v>4800</v>
+        <v>4900</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:12">
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="E29">
+        <v>3</v>
+      </c>
       <c r="F29">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="G29">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H29">
-        <v>4900</v>
+        <v>800</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:12">
       <c r="D30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E30">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F30">
         <v>3</v>
@@ -1304,67 +1325,46 @@
         <v>8</v>
       </c>
       <c r="H30">
-        <v>800</v>
+        <v>1000</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:12">
-      <c r="D31">
-        <v>1</v>
-      </c>
       <c r="E31">
         <v>4</v>
       </c>
       <c r="F31">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G31">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="H31">
-        <v>1000</v>
+        <v>1200</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:12">
       <c r="E32">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F32">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G32">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="H32">
-        <v>1200</v>
+        <v>1400</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="33" spans="5:9">
-      <c r="E33">
-        <v>3</v>
-      </c>
-      <c r="F33">
-        <v>5</v>
-      </c>
-      <c r="G33">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H33">
-        <v>1400</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test: modified calculation error
</commit_message>
<xml_diff>
--- a/PiratenKapern/src/test/java/test/game/Theme/theme test case.xlsx
+++ b/PiratenKapern/src/test/java/test/game/Theme/theme test case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Carleton\4004\a1\4004F2020-PiratenKapern\PiratenKapern\src\test\java\test\game\Theme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB32FC4-9545-4926-BC40-0D888C3AC16F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67CB9201-172A-4814-BF52-B9B1AE92F85D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="4485" windowWidth="20730" windowHeight="11160" xr2:uid="{4453D95F-B99C-4EBC-BF1D-88ACF2A1429C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
   <si>
     <t>Monkey</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -56,10 +56,6 @@
   </si>
   <si>
     <t>Diamond</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sum</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -670,19 +666,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F6EA3C4-DE68-497B-AA93-69DD73F51F1B}">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G15" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="8" max="8" width="18.375" customWidth="1"/>
-    <col min="9" max="9" width="41.375" customWidth="1"/>
+    <col min="7" max="7" width="18.375" customWidth="1"/>
+    <col min="8" max="8" width="41.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -702,16 +698,13 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="H1" t="s">
         <v>25</v>
       </c>
-      <c r="I1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -719,12 +712,11 @@
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="H2" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>3</v>
       </c>
@@ -744,15 +736,11 @@
         <v>1</v>
       </c>
       <c r="G3">
-        <f>SUM(A3:F3)</f>
-        <v>8</v>
-      </c>
-      <c r="H3">
         <v>0</v>
       </c>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>4</v>
       </c>
@@ -763,15 +751,11 @@
         <v>2</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G32" si="0">SUM(A4:F4)</f>
-        <v>8</v>
-      </c>
-      <c r="H4">
         <v>0</v>
       </c>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>2</v>
       </c>
@@ -785,17 +769,13 @@
         <v>1</v>
       </c>
       <c r="G5">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H5">
         <v>100</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="H5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>2</v>
       </c>
@@ -809,17 +789,13 @@
         <v>1</v>
       </c>
       <c r="G6">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H6">
         <v>200</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="H6" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>2</v>
       </c>
@@ -830,17 +806,13 @@
         <v>1</v>
       </c>
       <c r="G7">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H7">
         <v>500</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="H7" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>2</v>
       </c>
@@ -848,17 +820,13 @@
         <v>6</v>
       </c>
       <c r="G8">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H8">
         <v>1000</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="H8" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>1</v>
       </c>
@@ -866,32 +834,24 @@
         <v>7</v>
       </c>
       <c r="G9">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H9">
         <v>2000</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="H9" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="B10">
         <v>8</v>
       </c>
       <c r="G10">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H10">
         <v>4000</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="15" thickBot="1">
+      <c r="H10" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15" thickBot="1">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -899,12 +859,11 @@
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="H11" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12">
         <v>1</v>
       </c>
@@ -924,23 +883,19 @@
         <v>1</v>
       </c>
       <c r="G12">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H12">
         <v>300</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="L12" s="3">
+      <c r="H12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K12" s="3">
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:11">
       <c r="B13">
         <v>4</v>
       </c>
@@ -951,23 +906,19 @@
         <v>2</v>
       </c>
       <c r="G13">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H13">
         <v>600</v>
       </c>
-      <c r="I13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="L13" s="5">
+      <c r="H13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K13" s="5">
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:11">
       <c r="B14">
         <v>5</v>
       </c>
@@ -978,23 +929,19 @@
         <v>2</v>
       </c>
       <c r="G14">
-        <f t="shared" si="0"/>
+        <v>700</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H14">
-        <v>700</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="L14" s="5">
+      <c r="K14" s="5">
         <v>500</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:11">
       <c r="B15">
         <v>6</v>
       </c>
@@ -1005,23 +952,19 @@
         <v>1</v>
       </c>
       <c r="G15">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H15">
         <v>1100</v>
       </c>
-      <c r="I15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L15" s="5">
+      <c r="H15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K15" s="5">
         <v>1000</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:11">
       <c r="B16">
         <v>7</v>
       </c>
@@ -1029,23 +972,19 @@
         <v>1</v>
       </c>
       <c r="G16">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H16">
         <v>2100</v>
       </c>
-      <c r="I16" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="L16" s="5">
+      <c r="H16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K16" s="5">
         <v>2000</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:11">
       <c r="B17">
         <v>8</v>
       </c>
@@ -1053,23 +992,19 @@
         <v>1</v>
       </c>
       <c r="G17">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="H17">
         <v>4100</v>
       </c>
-      <c r="I17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K17" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="L17" s="5">
+      <c r="H17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K17" s="5">
         <v>4000</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="15" thickBot="1">
+    <row r="18" spans="1:11" ht="15" thickBot="1">
       <c r="A18">
         <v>2</v>
       </c>
@@ -1080,23 +1015,19 @@
         <v>3</v>
       </c>
       <c r="G18">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H18">
         <v>200</v>
       </c>
-      <c r="I18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K18" s="6" t="s">
+      <c r="H18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K18" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="L18" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1107,17 +1038,13 @@
         <v>4</v>
       </c>
       <c r="G19">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H19">
         <v>300</v>
       </c>
-      <c r="I19" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
+      <c r="H19" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="B20">
         <v>4</v>
       </c>
@@ -1125,17 +1052,13 @@
         <v>4</v>
       </c>
       <c r="G20">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H20">
         <v>400</v>
       </c>
-      <c r="I20" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
+      <c r="H20" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
@@ -1143,12 +1066,11 @@
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
+      <c r="H21" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1162,17 +1084,13 @@
         <v>3</v>
       </c>
       <c r="G22">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H22">
         <v>400</v>
       </c>
-      <c r="I22" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
+      <c r="H22" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1186,17 +1104,13 @@
         <v>4</v>
       </c>
       <c r="G23">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H23">
         <v>600</v>
       </c>
-      <c r="I23" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
+      <c r="H23" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1210,17 +1124,13 @@
         <v>5</v>
       </c>
       <c r="G24">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H24">
         <v>1000</v>
       </c>
-      <c r="I24" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
+      <c r="H24" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25">
         <v>1</v>
       </c>
@@ -1231,17 +1141,13 @@
         <v>6</v>
       </c>
       <c r="G25">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H25">
         <v>1600</v>
       </c>
-      <c r="I25" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
+      <c r="H25" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
       <c r="B26">
         <v>1</v>
       </c>
@@ -1249,47 +1155,35 @@
         <v>7</v>
       </c>
       <c r="G26">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H26">
         <v>2700</v>
       </c>
-      <c r="I26" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12">
+      <c r="H26" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
       <c r="F27">
         <v>8</v>
       </c>
       <c r="G27">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H27">
         <v>4800</v>
       </c>
-      <c r="I27" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12">
+      <c r="H27" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
       <c r="F28">
         <v>9</v>
       </c>
       <c r="G28">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="H28">
         <v>4900</v>
       </c>
-      <c r="I28" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12">
+      <c r="H28" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
       <c r="D29">
         <v>2</v>
       </c>
@@ -1300,17 +1194,13 @@
         <v>3</v>
       </c>
       <c r="G29">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H29">
         <v>800</v>
       </c>
-      <c r="I29" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12">
+      <c r="H29" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
       <c r="D30">
         <v>1</v>
       </c>
@@ -1321,17 +1211,13 @@
         <v>3</v>
       </c>
       <c r="G30">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H30">
         <v>1000</v>
       </c>
-      <c r="I30" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12">
+      <c r="H30" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
       <c r="E31">
         <v>4</v>
       </c>
@@ -1339,17 +1225,13 @@
         <v>4</v>
       </c>
       <c r="G31">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H31">
         <v>1200</v>
       </c>
-      <c r="I31" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12">
+      <c r="H31" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
       <c r="E32">
         <v>3</v>
       </c>
@@ -1357,14 +1239,10 @@
         <v>5</v>
       </c>
       <c r="G32">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H32">
         <v>1400</v>
       </c>
-      <c r="I32" s="1" t="s">
-        <v>39</v>
+      <c r="H32" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Other: update test tables regarding to the Full Chest Rull
</commit_message>
<xml_diff>
--- a/PiratenKapern/src/test/java/test/game/Theme/theme test case.xlsx
+++ b/PiratenKapern/src/test/java/test/game/Theme/theme test case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Carleton\4004\a1\4004F2020-PiratenKapern\PiratenKapern\src\test\java\test\game\Theme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67CB9201-172A-4814-BF52-B9B1AE92F85D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4506FF-8356-4C9B-AA65-A347E5E16B28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="4485" windowWidth="20730" windowHeight="11160" xr2:uid="{4453D95F-B99C-4EBC-BF1D-88ACF2A1429C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
   <si>
     <t>Monkey</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -91,10 +91,6 @@
     <t>8oak</t>
   </si>
   <si>
-    <t>8oak</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Coin/Dia</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -119,14 +115,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>7oak+coinx1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>8oak+coinx1(from fortune card)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>expect score</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -143,10 +131,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>4oakx2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>3oak+coinx3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -163,14 +147,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>8oak+coinx8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>8oak+coinx9(from fortune card)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>3oakx2+coinx6</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -179,14 +155,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>4oakx2+coinx8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3oak+5oak+coinx8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>no coin/diamond bonus</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -196,6 +164,66 @@
   </si>
   <si>
     <t>coin/diamond oak + bonus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>skulls from card</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Full Chest</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8oak+FC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4oak+coinx4+FC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7oak+coinx1+FC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8oak+coinx1(from fortune card)+FC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4oakx2+FC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8oak+coinx8+FC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8oak+coinx9(from fortune card)+FC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4oakx2+coinx8+FC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3oak+5oak+coinx8+FC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>skull from card</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8oak+FC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7oak</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5oak+coinx3+FC</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -225,7 +253,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -241,6 +269,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -321,7 +355,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -340,17 +374,23 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -666,19 +706,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F6EA3C4-DE68-497B-AA93-69DD73F51F1B}">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G15" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="7" max="7" width="18.375" customWidth="1"/>
-    <col min="8" max="8" width="41.375" customWidth="1"/>
+    <col min="7" max="8" width="18.375" customWidth="1"/>
+    <col min="9" max="9" width="41.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -698,25 +738,29 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+        <v>34</v>
+      </c>
+      <c r="I1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3">
         <v>3</v>
       </c>
@@ -738,9 +782,9 @@
       <c r="G3">
         <v>0</v>
       </c>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4">
         <v>4</v>
       </c>
@@ -753,9 +797,9 @@
       <c r="G4">
         <v>0</v>
       </c>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5">
         <v>2</v>
       </c>
@@ -771,11 +815,11 @@
       <c r="G5">
         <v>100</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:12">
       <c r="A6">
         <v>2</v>
       </c>
@@ -791,11 +835,11 @@
       <c r="G6">
         <v>200</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:12">
       <c r="A7">
         <v>2</v>
       </c>
@@ -808,11 +852,11 @@
       <c r="G7">
         <v>500</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:12">
       <c r="A8">
         <v>2</v>
       </c>
@@ -822,11 +866,11 @@
       <c r="G8">
         <v>1000</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:12">
       <c r="A9">
         <v>1</v>
       </c>
@@ -836,34 +880,35 @@
       <c r="G9">
         <v>2000</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:12">
       <c r="B10">
         <v>8</v>
       </c>
-      <c r="G10">
-        <v>4000</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="15" thickBot="1">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+      <c r="G10" s="11">
+        <v>4500</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15" thickBot="1">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12">
         <v>1</v>
       </c>
@@ -885,17 +930,17 @@
       <c r="G12">
         <v>300</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J12" s="2" t="s">
+      <c r="I12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K12" s="3">
+      <c r="L12" s="3">
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:12">
       <c r="B13">
         <v>4</v>
       </c>
@@ -905,20 +950,20 @@
       <c r="F13">
         <v>2</v>
       </c>
-      <c r="G13">
-        <v>600</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J13" s="4" t="s">
+      <c r="G13" s="11">
+        <v>1100</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K13" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K13" s="5">
+      <c r="L13" s="5">
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:12">
       <c r="B14">
         <v>5</v>
       </c>
@@ -931,17 +976,17 @@
       <c r="G14">
         <v>700</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J14" s="4" t="s">
+      <c r="I14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K14" s="5">
+      <c r="L14" s="5">
         <v>500</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:12">
       <c r="B15">
         <v>6</v>
       </c>
@@ -954,57 +999,57 @@
       <c r="G15">
         <v>1100</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J15" s="4" t="s">
+      <c r="I15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K15" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K15" s="5">
+      <c r="L15" s="5">
         <v>1000</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:12">
       <c r="B16">
         <v>7</v>
       </c>
       <c r="F16">
         <v>1</v>
       </c>
-      <c r="G16">
-        <v>2100</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J16" s="4" t="s">
+      <c r="G16" s="11">
+        <v>2600</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K16" s="5">
+      <c r="L16" s="5">
         <v>2000</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:12">
       <c r="B17">
         <v>8</v>
       </c>
       <c r="F17">
         <v>1</v>
       </c>
-      <c r="G17">
-        <v>4100</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J17" s="4" t="s">
+      <c r="G17" s="11">
+        <v>4600</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K17" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K17" s="5">
+      <c r="L17" s="5">
         <v>4000</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="15" thickBot="1">
+    <row r="18" spans="1:12">
       <c r="A18">
         <v>2</v>
       </c>
@@ -1017,17 +1062,17 @@
       <c r="G18">
         <v>200</v>
       </c>
-      <c r="H18" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J18" s="6" t="s">
+      <c r="I18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L18" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="K18" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
+    </row>
+    <row r="19" spans="1:12" ht="15" thickBot="1">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1040,37 +1085,44 @@
       <c r="G19">
         <v>300</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
+      <c r="I19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="L19" s="9">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="B20">
         <v>4</v>
       </c>
       <c r="C20">
         <v>4</v>
       </c>
-      <c r="G20">
-        <v>400</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
+      <c r="G20" s="11">
+        <v>900</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1086,11 +1138,11 @@
       <c r="G22">
         <v>400</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
+      <c r="I22" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1106,11 +1158,11 @@
       <c r="G23">
         <v>600</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
+      <c r="I23" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1126,11 +1178,11 @@
       <c r="G24">
         <v>1000</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11">
+      <c r="I24" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25">
         <v>1</v>
       </c>
@@ -1143,11 +1195,11 @@
       <c r="G25">
         <v>1600</v>
       </c>
-      <c r="H25" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11">
+      <c r="I25" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
       <c r="B26">
         <v>1</v>
       </c>
@@ -1157,33 +1209,33 @@
       <c r="G26">
         <v>2700</v>
       </c>
-      <c r="H26" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
+      <c r="I26" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
       <c r="F27">
         <v>8</v>
       </c>
-      <c r="G27">
-        <v>4800</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11">
+      <c r="G27" s="11">
+        <v>5300</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
       <c r="F28">
         <v>9</v>
       </c>
-      <c r="G28">
-        <v>4900</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11">
+      <c r="G28" s="11">
+        <v>5400</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
       <c r="D29">
         <v>2</v>
       </c>
@@ -1196,11 +1248,11 @@
       <c r="G29">
         <v>800</v>
       </c>
-      <c r="H29" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11">
+      <c r="I29" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
       <c r="D30">
         <v>1</v>
       </c>
@@ -1213,36 +1265,100 @@
       <c r="G30">
         <v>1000</v>
       </c>
-      <c r="H30" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11">
+      <c r="I30" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
       <c r="E31">
         <v>4</v>
       </c>
       <c r="F31">
         <v>4</v>
       </c>
-      <c r="G31">
-        <v>1200</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11">
+      <c r="G31" s="11">
+        <v>1700</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
       <c r="E32">
         <v>3</v>
       </c>
       <c r="F32">
         <v>5</v>
       </c>
-      <c r="G32">
-        <v>1400</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>38</v>
+      <c r="G32" s="11">
+        <v>1900</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="B34">
+        <v>8</v>
+      </c>
+      <c r="G34">
+        <v>4500</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35">
+        <v>7</v>
+      </c>
+      <c r="G35">
+        <v>2000</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="B36">
+        <v>5</v>
+      </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36">
+        <v>1300</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test: modified test case for Normal theme   -Full Chest rule applied
</commit_message>
<xml_diff>
--- a/PiratenKapern/src/test/java/test/game/Theme/theme test case.xlsx
+++ b/PiratenKapern/src/test/java/test/game/Theme/theme test case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Carleton\4004\a1\4004F2020-PiratenKapern\PiratenKapern\src\test\java\test\game\Theme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4506FF-8356-4C9B-AA65-A347E5E16B28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BEAB4D3-71F7-4367-87C6-9C08F89024E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="4485" windowWidth="20730" windowHeight="11160" xr2:uid="{4453D95F-B99C-4EBC-BF1D-88ACF2A1429C}"/>
   </bookViews>
@@ -33,16 +33,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
   <si>
     <t>Monkey</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Skull</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Parrot</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -224,6 +220,18 @@
   </si>
   <si>
     <t>5oak+coinx3+FC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6oak</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Skull total</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Check</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -706,45 +714,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F6EA3C4-DE68-497B-AA93-69DD73F51F1B}">
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
+    <col min="1" max="1" width="18.625" customWidth="1"/>
     <col min="7" max="8" width="18.375" customWidth="1"/>
     <col min="9" max="9" width="41.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
       <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" t="s">
-        <v>22</v>
+      <c r="J1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -757,7 +769,7 @@
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -783,6 +795,10 @@
         <v>0</v>
       </c>
       <c r="I3" s="1"/>
+      <c r="J3">
+        <f>SUM(A3:F3)-H3</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4">
@@ -798,6 +814,10 @@
         <v>0</v>
       </c>
       <c r="I4" s="1"/>
+      <c r="J4">
+        <f t="shared" ref="J4:J37" si="0">SUM(A4:F4)-H4</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5">
@@ -816,7 +836,11 @@
         <v>100</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -836,7 +860,11 @@
         <v>200</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -853,7 +881,11 @@
         <v>500</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -867,7 +899,11 @@
         <v>1000</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -881,7 +917,11 @@
         <v>2000</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -892,7 +932,11 @@
         <v>4500</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="15" thickBot="1">
@@ -905,7 +949,7 @@
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -931,10 +975,14 @@
         <v>300</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L12" s="3">
         <v>100</v>
@@ -954,10 +1002,14 @@
         <v>1100</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L13" s="5">
         <v>200</v>
@@ -977,10 +1029,14 @@
         <v>700</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L14" s="5">
         <v>500</v>
@@ -1000,10 +1056,14 @@
         <v>1100</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L15" s="5">
         <v>1000</v>
@@ -1020,10 +1080,14 @@
         <v>2600</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L16" s="5">
         <v>2000</v>
@@ -1040,10 +1104,14 @@
         <v>4600</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L17" s="5">
         <v>4000</v>
@@ -1063,13 +1131,17 @@
         <v>200</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
       <c r="K18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L18" s="10" t="s">
         <v>15</v>
-      </c>
-      <c r="L18" s="10" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="15" thickBot="1">
@@ -1086,10 +1158,14 @@
         <v>300</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L19" s="9">
         <v>500</v>
@@ -1106,7 +1182,11 @@
         <v>900</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1119,7 +1199,7 @@
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
       <c r="I21" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -1139,7 +1219,11 @@
         <v>400</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -1159,7 +1243,11 @@
         <v>600</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -1179,7 +1267,11 @@
         <v>1000</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -1196,7 +1288,11 @@
         <v>1600</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -1210,7 +1306,11 @@
         <v>2700</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -1221,7 +1321,11 @@
         <v>5300</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -1232,7 +1336,11 @@
         <v>5400</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -1249,7 +1357,11 @@
         <v>800</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -1266,7 +1378,11 @@
         <v>1000</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -1280,7 +1396,11 @@
         <v>1700</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -1294,10 +1414,14 @@
         <v>1900</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
+        <v>43</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
@@ -1307,10 +1431,13 @@
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
       <c r="I33" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34">
+        <v>1</v>
+      </c>
       <c r="B34">
         <v>8</v>
       </c>
@@ -1321,12 +1448,16 @@
         <v>1</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
+        <v>45</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B35">
         <v>7</v>
@@ -1335,13 +1466,20 @@
         <v>2000</v>
       </c>
       <c r="H35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
+        <v>46</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36">
+        <v>1</v>
+      </c>
       <c r="B36">
         <v>5</v>
       </c>
@@ -1358,7 +1496,38 @@
         <v>1</v>
       </c>
       <c r="I36" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37">
+        <v>2</v>
+      </c>
+      <c r="B37">
+        <v>6</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="G37">
+        <v>1000</v>
+      </c>
+      <c r="H37">
+        <v>2</v>
+      </c>
+      <c r="I37" s="1" t="s">
         <v>48</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Other: update test table for SkullIsland theme
</commit_message>
<xml_diff>
--- a/PiratenKapern/src/test/java/test/game/Theme/theme test case.xlsx
+++ b/PiratenKapern/src/test/java/test/game/Theme/theme test case.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Carleton\4004\a1\4004F2020-PiratenKapern\PiratenKapern\src\test\java\test\game\Theme\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haiyuesun/Desktop/4004/a1/4004F2020-PiratenKapern/PiratenKapern/src/test/java/test/game/Theme/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BEAB4D3-71F7-4367-87C6-9C08F89024E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB51F062-A085-B146-8015-8847049A9BA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="4485" windowWidth="20730" windowHeight="11160" xr2:uid="{4453D95F-B99C-4EBC-BF1D-88ACF2A1429C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" activeTab="1" xr2:uid="{4453D95F-B99C-4EBC-BF1D-88ACF2A1429C}"/>
   </bookViews>
   <sheets>
     <sheet name="Normal" sheetId="1" r:id="rId1"/>
+    <sheet name="SkullIsland" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="54">
   <si>
     <t>Monkey</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -232,6 +233,18 @@
   </si>
   <si>
     <t>Check</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Skull</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>expect</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sum check</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -258,6 +271,7 @@
     <font>
       <sz val="11"/>
       <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -716,15 +730,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F6EA3C4-DE68-497B-AA93-69DD73F51F1B}">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.625" customWidth="1"/>
-    <col min="7" max="8" width="18.375" customWidth="1"/>
-    <col min="9" max="9" width="41.375" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="7" max="8" width="18.33203125" customWidth="1"/>
+    <col min="9" max="9" width="41.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -939,7 +953,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15" thickBot="1">
+    <row r="11" spans="1:12" ht="16" thickBot="1">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -1144,7 +1158,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15" thickBot="1">
+    <row r="19" spans="1:12" ht="16" thickBot="1">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1535,4 +1549,236 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{612D2292-9E3F-854E-B6CA-2E8E07F34F73}">
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="7" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <f>A2 * (-100)</f>
+        <v>-100</v>
+      </c>
+      <c r="I2">
+        <f>SUM(A2:F2)-H2</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G11" si="0">A3 * (-100)</f>
+        <v>-200</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I11" si="1">SUM(A3:F3)-H3</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>-300</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>-400</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>-500</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>-600</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>-700</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>-800</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>-900</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>-1000</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Other: add test table for MonkeyBussiness Theme
</commit_message>
<xml_diff>
--- a/PiratenKapern/src/test/java/test/game/Theme/theme test case.xlsx
+++ b/PiratenKapern/src/test/java/test/game/Theme/theme test case.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haiyuesun/Desktop/4004/a1/4004F2020-PiratenKapern/PiratenKapern/src/test/java/test/game/Theme/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB51F062-A085-B146-8015-8847049A9BA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{355FD5C3-4276-AA43-B52F-B08FE87BCFB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" activeTab="1" xr2:uid="{4453D95F-B99C-4EBC-BF1D-88ACF2A1429C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" activeTab="2" xr2:uid="{4453D95F-B99C-4EBC-BF1D-88ACF2A1429C}"/>
   </bookViews>
   <sheets>
     <sheet name="Normal" sheetId="1" r:id="rId1"/>
     <sheet name="SkullIsland" sheetId="2" r:id="rId2"/>
+    <sheet name="MonkeyBusiness" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="56">
   <si>
     <t>Monkey</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -245,6 +246,14 @@
   </si>
   <si>
     <t>sum check</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>coinx2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3oak+coin</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1555,8 +1564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{612D2292-9E3F-854E-B6CA-2E8E07F34F73}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1781,4 +1790,275 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1070585C-640B-DA46-8DF8-77CFA5F1FE16}">
+  <dimension ref="A1:J10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I11:I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>200</v>
+      </c>
+      <c r="I2">
+        <f>SUM(A2:F2)</f>
+        <v>8</v>
+      </c>
+      <c r="J2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>200</v>
+      </c>
+      <c r="I3">
+        <f>SUM(A3:F3)</f>
+        <v>8</v>
+      </c>
+      <c r="J3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>200</v>
+      </c>
+      <c r="I4">
+        <f>SUM(A4:F4)</f>
+        <v>8</v>
+      </c>
+      <c r="J4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>200</v>
+      </c>
+      <c r="I5">
+        <f>SUM(A5:F5)</f>
+        <v>8</v>
+      </c>
+      <c r="J5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>500</v>
+      </c>
+      <c r="I6">
+        <f>SUM(A6:F6)</f>
+        <v>8</v>
+      </c>
+      <c r="J6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <v>1000</v>
+      </c>
+      <c r="I7">
+        <f t="shared" ref="I3:I14" si="0">SUM(A7:F7)</f>
+        <v>8</v>
+      </c>
+      <c r="J7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="G8">
+        <v>2000</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="J8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="G9">
+        <v>5500</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="J9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>1300</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="J10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Other: add test table for SeaBattle theme
</commit_message>
<xml_diff>
--- a/PiratenKapern/src/test/java/test/game/Theme/theme test case.xlsx
+++ b/PiratenKapern/src/test/java/test/game/Theme/theme test case.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haiyuesun/Desktop/4004/a1/4004F2020-PiratenKapern/PiratenKapern/src/test/java/test/game/Theme/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{355FD5C3-4276-AA43-B52F-B08FE87BCFB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E120772-D84C-1F4F-97D9-79F23BBD34F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" activeTab="2" xr2:uid="{4453D95F-B99C-4EBC-BF1D-88ACF2A1429C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" activeTab="3" xr2:uid="{4453D95F-B99C-4EBC-BF1D-88ACF2A1429C}"/>
   </bookViews>
   <sheets>
     <sheet name="Normal" sheetId="1" r:id="rId1"/>
     <sheet name="SkullIsland" sheetId="2" r:id="rId2"/>
     <sheet name="MonkeyBusiness" sheetId="3" r:id="rId3"/>
+    <sheet name="SeaBattle" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="65">
   <si>
     <t>Monkey</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -254,6 +255,42 @@
   </si>
   <si>
     <t>3oak+coin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sword require</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reward</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>defeat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>victory+3oak+coinx3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>victory+3oakx2+coinx5+FC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>victory+3oakx2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>victory+4oak+coinx4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>victory+4oak</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>victory+5oak+coinx3+FC</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -739,8 +776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F6EA3C4-DE68-497B-AA93-69DD73F51F1B}">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1796,8 +1833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1070585C-640B-DA46-8DF8-77CFA5F1FE16}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I11:I14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2061,4 +2098,307 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A6B09B5-66AA-0E43-A75A-E7557F66FF3A}">
+  <dimension ref="A1:K10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" customWidth="1"/>
+    <col min="9" max="9" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>-100</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>100</v>
+      </c>
+      <c r="J2" t="s">
+        <v>58</v>
+      </c>
+      <c r="K2">
+        <f>SUM(A2:F2)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>500</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>100</v>
+      </c>
+      <c r="J3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K10" si="0">SUM(A3:F3)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>1300</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>100</v>
+      </c>
+      <c r="J4" t="s">
+        <v>60</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>-200</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>200</v>
+      </c>
+      <c r="J5" t="s">
+        <v>58</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>400</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <v>200</v>
+      </c>
+      <c r="J6" t="s">
+        <v>61</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>800</v>
+      </c>
+      <c r="H7">
+        <v>3</v>
+      </c>
+      <c r="I7">
+        <v>200</v>
+      </c>
+      <c r="J7" t="s">
+        <v>62</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="G8">
+        <v>-500</v>
+      </c>
+      <c r="H8">
+        <v>4</v>
+      </c>
+      <c r="I8">
+        <v>500</v>
+      </c>
+      <c r="J8" t="s">
+        <v>58</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="G9">
+        <v>700</v>
+      </c>
+      <c r="H9">
+        <v>4</v>
+      </c>
+      <c r="I9">
+        <v>500</v>
+      </c>
+      <c r="J9" t="s">
+        <v>63</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>1800</v>
+      </c>
+      <c r="H10">
+        <v>4</v>
+      </c>
+      <c r="I10">
+        <v>500</v>
+      </c>
+      <c r="J10" t="s">
+        <v>64</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Test: fix the calculation mistake   -Coin/Diamond bonus was not considered in test_3_sabre tese case[1]   -Full Chest was not considered in test_3_sabre test case[2]
</commit_message>
<xml_diff>
--- a/PiratenKapern/src/test/java/test/game/Theme/theme test case.xlsx
+++ b/PiratenKapern/src/test/java/test/game/Theme/theme test case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haiyuesun/Desktop/4004/a1/4004F2020-PiratenKapern/PiratenKapern/src/test/java/test/game/Theme/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E120772-D84C-1F4F-97D9-79F23BBD34F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A9B54D-1D4A-D047-BD9A-C67862F78D9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" activeTab="3" xr2:uid="{4453D95F-B99C-4EBC-BF1D-88ACF2A1429C}"/>
   </bookViews>
@@ -278,19 +278,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>victory+3oakx2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>victory+4oak+coinx4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>victory+4oak</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>victory+5oak+coinx3+FC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>victory+3oakx2+coinx3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>victory+4oak+coinx4+FC</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2105,7 +2105,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2273,7 +2273,7 @@
         <v>3</v>
       </c>
       <c r="G6">
-        <v>400</v>
+        <v>700</v>
       </c>
       <c r="H6">
         <v>3</v>
@@ -2282,7 +2282,7 @@
         <v>200</v>
       </c>
       <c r="J6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="K6">
         <f t="shared" si="0"/>
@@ -2300,7 +2300,7 @@
         <v>2</v>
       </c>
       <c r="G7">
-        <v>800</v>
+        <v>1300</v>
       </c>
       <c r="H7">
         <v>3</v>
@@ -2309,7 +2309,7 @@
         <v>200</v>
       </c>
       <c r="J7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K7">
         <f t="shared" si="0"/>
@@ -2363,7 +2363,7 @@
         <v>500</v>
       </c>
       <c r="J9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K9">
         <f t="shared" si="0"/>
@@ -2390,7 +2390,7 @@
         <v>500</v>
       </c>
       <c r="J10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K10">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
bug fix: score calculation fixed regarding to the rule
</commit_message>
<xml_diff>
--- a/PiratenKapern/src/test/java/test/game/Theme/theme test case.xlsx
+++ b/PiratenKapern/src/test/java/test/game/Theme/theme test case.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haiyuesun/Desktop/4004/a1/4004F2020-PiratenKapern/PiratenKapern/src/test/java/test/game/Theme/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Carleton\4004\a1\4004F2020-PiratenKapern\PiratenKapern\src\test\java\test\game\Theme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A9B54D-1D4A-D047-BD9A-C67862F78D9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74F10E9-0B2A-4BF9-A40B-FD46412A9E76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" activeTab="3" xr2:uid="{4453D95F-B99C-4EBC-BF1D-88ACF2A1429C}"/>
+    <workbookView xWindow="28680" yWindow="4485" windowWidth="20730" windowHeight="11160" xr2:uid="{4453D95F-B99C-4EBC-BF1D-88ACF2A1429C}"/>
   </bookViews>
   <sheets>
     <sheet name="Normal" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="MonkeyBusiness" sheetId="3" r:id="rId3"/>
     <sheet name="SeaBattle" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" refMode="R1C1" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -218,10 +218,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>7oak</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>5oak+coinx3+FC</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -291,6 +287,10 @@
   </si>
   <si>
     <t>victory+4oak+coinx4+FC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>disqualified</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -317,7 +317,6 @@
     <font>
       <sz val="11"/>
       <name val="等线"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -776,20 +775,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F6EA3C4-DE68-497B-AA93-69DD73F51F1B}">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="7" max="8" width="18.33203125" customWidth="1"/>
-    <col min="9" max="9" width="41.33203125" customWidth="1"/>
+    <col min="1" max="1" width="18.625" customWidth="1"/>
+    <col min="7" max="8" width="18.375" customWidth="1"/>
+    <col min="9" max="9" width="41.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -816,7 +815,7 @@
         <v>21</v>
       </c>
       <c r="J1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -999,7 +998,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="16" thickBot="1">
+    <row r="11" spans="1:12" ht="15" thickBot="1">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -1204,7 +1203,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="16" thickBot="1">
+    <row r="19" spans="1:12" ht="15" thickBot="1">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1523,13 +1522,13 @@
         <v>7</v>
       </c>
       <c r="G35">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="H35">
         <v>2</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="J35">
         <f t="shared" si="0"/>
@@ -1556,7 +1555,7 @@
         <v>1</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J36">
         <f t="shared" si="0"/>
@@ -1583,7 +1582,7 @@
         <v>2</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J37">
         <f t="shared" si="0"/>
@@ -1605,14 +1604,14 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
   <cols>
-    <col min="7" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1630,13 +1629,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H1" t="s">
         <v>44</v>
       </c>
       <c r="I1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1837,15 +1836,15 @@
       <selection activeCell="H2" sqref="H2:H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
   <cols>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1863,13 +1862,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H1" t="s">
         <v>44</v>
       </c>
       <c r="I1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J1" t="s">
         <v>21</v>
@@ -1902,7 +1901,7 @@
         <v>8</v>
       </c>
       <c r="J2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1929,7 +1928,7 @@
         <v>8</v>
       </c>
       <c r="J3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1956,7 +1955,7 @@
         <v>8</v>
       </c>
       <c r="J4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -2021,7 +2020,7 @@
         <v>1000</v>
       </c>
       <c r="I7">
-        <f t="shared" ref="I3:I14" si="0">SUM(A7:F7)</f>
+        <f t="shared" ref="I7:I10" si="0">SUM(A7:F7)</f>
         <v>8</v>
       </c>
       <c r="J7" t="s">
@@ -2091,7 +2090,7 @@
         <v>8</v>
       </c>
       <c r="J10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -2104,21 +2103,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A6B09B5-66AA-0E43-A75A-E7557F66FF3A}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
   <cols>
-    <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.83203125" customWidth="1"/>
-    <col min="9" max="9" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.33203125" customWidth="1"/>
+    <col min="7" max="7" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.875" customWidth="1"/>
+    <col min="9" max="9" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2139,16 +2138,16 @@
         <v>20</v>
       </c>
       <c r="H1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" t="s">
         <v>56</v>
-      </c>
-      <c r="I1" t="s">
-        <v>57</v>
       </c>
       <c r="J1" t="s">
         <v>21</v>
       </c>
       <c r="K1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -2171,7 +2170,7 @@
         <v>100</v>
       </c>
       <c r="J2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K2">
         <f>SUM(A2:F2)</f>
@@ -2201,7 +2200,7 @@
         <v>100</v>
       </c>
       <c r="J3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K3">
         <f t="shared" ref="K3:K10" si="0">SUM(A3:F3)</f>
@@ -2228,7 +2227,7 @@
         <v>100</v>
       </c>
       <c r="J4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K4">
         <f t="shared" si="0"/>
@@ -2255,7 +2254,7 @@
         <v>200</v>
       </c>
       <c r="J5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K5">
         <f t="shared" si="0"/>
@@ -2282,7 +2281,7 @@
         <v>200</v>
       </c>
       <c r="J6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K6">
         <f t="shared" si="0"/>
@@ -2309,7 +2308,7 @@
         <v>200</v>
       </c>
       <c r="J7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K7">
         <f t="shared" si="0"/>
@@ -2336,7 +2335,7 @@
         <v>500</v>
       </c>
       <c r="J8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K8">
         <f t="shared" si="0"/>
@@ -2363,7 +2362,7 @@
         <v>500</v>
       </c>
       <c r="J9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K9">
         <f t="shared" si="0"/>
@@ -2390,7 +2389,7 @@
         <v>500</v>
       </c>
       <c r="J10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K10">
         <f t="shared" si="0"/>

</xml_diff>